<commit_message>
include final lung datasets This commit is before migrating to seurat V5
</commit_message>
<xml_diff>
--- a/Mined_Data.xlsx
+++ b/Mined_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexwhitehead/Documents/Postdoc/Bl_Eng2_Priming/Vax_PRRs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3314E7F8-D0B4-4F44-8D32-8B42967CC60F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D577B5AB-D420-A947-8737-9C8029D3A43C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23800" yWindow="760" windowWidth="10760" windowHeight="19840" xr2:uid="{EE833336-1921-064D-BC1E-2DF7FFE7A9DF}"/>
+    <workbookView xWindow="17440" yWindow="760" windowWidth="17120" windowHeight="19840" xr2:uid="{EE833336-1921-064D-BC1E-2DF7FFE7A9DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Datasets Used" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="45">
-  <si>
-    <t>GEO/EGA Accession</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="59">
   <si>
     <t>Author</t>
   </si>
@@ -171,6 +168,51 @@
   </si>
   <si>
     <t>Seurat</t>
+  </si>
+  <si>
+    <t>Muscle</t>
+  </si>
+  <si>
+    <t>Is integrated from 20 sc/sn datasets across 111 samples,</t>
+  </si>
+  <si>
+    <t>doi:10.5061/dryad.t4b8gtj34</t>
+  </si>
+  <si>
+    <t>McKellar/Cosgrove</t>
+  </si>
+  <si>
+    <t>SC+ SN</t>
+  </si>
+  <si>
+    <t>365k</t>
+  </si>
+  <si>
+    <t>209k</t>
+  </si>
+  <si>
+    <t>Eraslan/Regev</t>
+  </si>
+  <si>
+    <t>16 donors</t>
+  </si>
+  <si>
+    <t>SCP1479</t>
+  </si>
+  <si>
+    <t>31k</t>
+  </si>
+  <si>
+    <t>5 donors</t>
+  </si>
+  <si>
+    <t>Quake</t>
+  </si>
+  <si>
+    <t>GEO/EGA Accession/Dryad/SingleCellPortal/HCAProject</t>
+  </si>
+  <si>
+    <t>10201832-7c73-4033-9b65-3ef13d81656a</t>
   </si>
 </sst>
 </file>
@@ -531,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{301386B4-EBD5-4C40-A49B-C59A5913FD6B}">
-  <dimension ref="A2:G20"/>
+  <dimension ref="A2:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -546,334 +588,403 @@
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" t="s">
-        <v>3</v>
-      </c>
       <c r="G2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" t="s">
         <v>20</v>
       </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" t="s">
-        <v>21</v>
-      </c>
       <c r="E10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" t="s">
         <v>26</v>
-      </c>
-      <c r="D14" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" t="s">
         <v>35</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>36</v>
       </c>
-      <c r="D15" t="s">
-        <v>37</v>
-      </c>
       <c r="E15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" t="s">
         <v>39</v>
-      </c>
-      <c r="D16" t="s">
-        <v>38</v>
-      </c>
-      <c r="E16" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" t="s">
         <v>39</v>
-      </c>
-      <c r="D17" t="s">
-        <v>38</v>
-      </c>
-      <c r="E17" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G18" t="s">
         <v>41</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G18" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" t="s">
         <v>43</v>
-      </c>
-      <c r="D19" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E20" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" t="s">
+        <v>50</v>
+      </c>
+      <c r="G21" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" t="s">
+        <v>47</v>
+      </c>
+      <c r="E22" t="s">
+        <v>48</v>
+      </c>
+      <c r="F22" t="s">
+        <v>49</v>
+      </c>
+      <c r="G22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" t="s">
+        <v>54</v>
+      </c>
+      <c r="G23" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>